<commit_message>
import convert entry and convert api entries to useable dicts. pass to filter. add save statement
</commit_message>
<xml_diff>
--- a/event_entries/master_entry_list.xlsx
+++ b/event_entries/master_entry_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brendanwoo/projects/sro_sign_in/event_entries/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C5B4058-E375-BA44-A91A-913FBD32082C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B1EDD64-00AE-E541-A061-AE20FE84622D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38400" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="34">
   <si>
     <t>id</t>
   </si>
@@ -119,6 +119,9 @@
   </si>
   <si>
     <t>2023-10-31T15:51:39Z</t>
+  </si>
+  <si>
+    <t>Mobil1</t>
   </si>
 </sst>
 </file>
@@ -614,7 +617,7 @@
   <dimension ref="A1:R33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="N12" sqref="N12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -732,7 +735,7 @@
         <v>29</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="O2" s="2" t="s">
         <v>25</v>

</xml_diff>